<commit_message>
change breast cancer wisconsin
</commit_message>
<xml_diff>
--- a/Breast_Cancer_Wisconsin/outputs/train_40_test_60/bcw_train_40_test_60_depth_accuracy.xlsx
+++ b/Breast_Cancer_Wisconsin/outputs/train_40_test_60/bcw_train_40_test_60_depth_accuracy.xlsx
@@ -461,10 +461,10 @@
         <v>0.9122807017543859</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9181286549707602</v>
+        <v>0.9327485380116959</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9181286549707602</v>
+        <v>0.9327485380116959</v>
       </c>
       <c r="E2" t="n">
         <v>0.9122807017543859</v>

</xml_diff>